<commit_message>
css: add box model and refine
</commit_message>
<xml_diff>
--- a/english/phrases.xlsx
+++ b/english/phrases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255"/>
+    <workbookView windowWidth="27945" windowHeight="12255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="word" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
   <si>
     <t>word</t>
   </si>
@@ -72,6 +72,24 @@
     <t>descendant</t>
   </si>
   <si>
+    <t>indices</t>
+  </si>
+  <si>
+    <t>/ˈɪndɪsiːz/</t>
+  </si>
+  <si>
+    <t>bind</t>
+  </si>
+  <si>
+    <t>/baɪnd/</t>
+  </si>
+  <si>
+    <t>bound</t>
+  </si>
+  <si>
+    <t>/baʊnd/</t>
+  </si>
+  <si>
     <t>Phrase</t>
   </si>
   <si>
@@ -622,6 +640,45 @@
   </si>
   <si>
     <t>You might have to resort to using inline styles if your working environment is very restrictive.</t>
+  </si>
+  <si>
+    <t>so much that</t>
+  </si>
+  <si>
+    <t>以至于</t>
+  </si>
+  <si>
+    <t>是一个常用的程度状语从句结构，用于强调前面所述动作或状态的极高程度，并表示这种程度所导致的直接结果</t>
+  </si>
+  <si>
+    <t>I'm a big fan of resetting box-sizing to border-box, so much that we have a special day of the year around here.</t>
+  </si>
+  <si>
+    <t>around here</t>
+  </si>
+  <si>
+    <t>在我们这儿</t>
+  </si>
+  <si>
+    <t>可以指物理区域：“Is there a good coffee shop around here?”，也可以指指工作或社交环境：“That’s how we do things around here.”。</t>
+  </si>
+  <si>
+    <t>credit on ... to sb</t>
+  </si>
+  <si>
+    <t>将关于（某事物）的功劳归于某人</t>
+  </si>
+  <si>
+    <t>Credit on the inheritance idea to Jon Neal.</t>
+  </si>
+  <si>
+    <t>bounded by</t>
+  </si>
+  <si>
+    <t>由/被…所界定</t>
+  </si>
+  <si>
+    <t>The margin area, bounded by the margin edge, extends the border area to include an empty area used to separate the element from its neighbors.</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1306,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1264,6 +1321,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1798,10 +1858,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -1870,6 +1930,30 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" ht="15" spans="1:2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" spans="1:2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1879,12 +1963,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -1897,680 +1981,728 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" ht="14.25" spans="1:3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" ht="40.5" spans="1:4">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" ht="27" spans="1:4">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D33" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C40" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B42" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" ht="14.25" spans="1:4">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="D50" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D51" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B52" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B54" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="B55" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B56" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B57" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D57" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B58" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B59" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C59" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D59" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B60" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C60" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B61" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B62" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C62" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D62" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B63" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>204</v>
+      </c>
+      <c r="B64" t="s">
+        <v>205</v>
+      </c>
+      <c r="C64" t="s">
+        <v>206</v>
+      </c>
+      <c r="D64" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C65" t="s">
+        <v>210</v>
+      </c>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>211</v>
+      </c>
+      <c r="B66" t="s">
+        <v>212</v>
+      </c>
+      <c r="D66" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>214</v>
+      </c>
+      <c r="B67" t="s">
+        <v>215</v>
+      </c>
+      <c r="D67" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
english: add words and phrases
</commit_message>
<xml_diff>
--- a/english/phrases.xlsx
+++ b/english/phrases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="310">
   <si>
     <t>word</t>
   </si>
@@ -138,6 +138,207 @@
     <t>/ˈælɡərɪðəm/</t>
   </si>
   <si>
+    <t>timely</t>
+  </si>
+  <si>
+    <t>idiosyncratic</t>
+  </si>
+  <si>
+    <t>/ˌɪdiəsɪŋˈkrætɪk/</t>
+  </si>
+  <si>
+    <t>parliament</t>
+  </si>
+  <si>
+    <t>/ˈpɑːrləmənt/</t>
+  </si>
+  <si>
+    <t>cellist</t>
+  </si>
+  <si>
+    <t>/ˈtʃelɪst/</t>
+  </si>
+  <si>
+    <t>facade</t>
+  </si>
+  <si>
+    <t>/fəˈsɑːd/</t>
+  </si>
+  <si>
+    <t>heir</t>
+  </si>
+  <si>
+    <t>/er/</t>
+  </si>
+  <si>
+    <t>niche</t>
+  </si>
+  <si>
+    <t>/niːʃ/</t>
+  </si>
+  <si>
+    <t>specific</t>
+  </si>
+  <si>
+    <t>/spəˈsɪfɪk/</t>
+  </si>
+  <si>
+    <t>penalty</t>
+  </si>
+  <si>
+    <t>/ˈpenəlti/</t>
+  </si>
+  <si>
+    <t>penalize</t>
+  </si>
+  <si>
+    <t>/ˈpiːnəlaɪz/</t>
+  </si>
+  <si>
+    <t>economy</t>
+  </si>
+  <si>
+    <t>/ɪˈkɑːnəmi/</t>
+  </si>
+  <si>
+    <t>economics</t>
+  </si>
+  <si>
+    <t>/ˌiːkəˈnɑːmɪks/</t>
+  </si>
+  <si>
+    <t>economist</t>
+  </si>
+  <si>
+    <t>/ɪˈkɑːnəmɪst/</t>
+  </si>
+  <si>
+    <t>debt</t>
+  </si>
+  <si>
+    <t>/det/</t>
+  </si>
+  <si>
+    <t>ichthyosaur</t>
+  </si>
+  <si>
+    <t>/ˈɪkθiəˌsɔːr/</t>
+  </si>
+  <si>
+    <t>resumé</t>
+  </si>
+  <si>
+    <t>/ˈrezəmeɪ/</t>
+  </si>
+  <si>
+    <t>resume</t>
+  </si>
+  <si>
+    <t>/rɪˈzuːm/</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>/kriˈeɪt/</t>
+  </si>
+  <si>
+    <t>reserve</t>
+  </si>
+  <si>
+    <t>/rɪˈzɜːrv/</t>
+  </si>
+  <si>
+    <t>reservation</t>
+  </si>
+  <si>
+    <t>/ˌrezərˈveɪʃ(ə)n/</t>
+  </si>
+  <si>
+    <t>conserve</t>
+  </si>
+  <si>
+    <t>/kənˈsɜːrv/</t>
+  </si>
+  <si>
+    <t>conservation</t>
+  </si>
+  <si>
+    <t>/ˌkɑːnsərˈveɪʃ(ə)n/</t>
+  </si>
+  <si>
+    <t>conservative</t>
+  </si>
+  <si>
+    <t>/kənˈsɜːrvətɪv/</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>/ˈɪzrɪəl/</t>
+  </si>
+  <si>
+    <t>cease</t>
+  </si>
+  <si>
+    <t>/siːs/</t>
+  </si>
+  <si>
+    <t>ceasefire</t>
+  </si>
+  <si>
+    <t>/ˈsiːsfaɪər/</t>
+  </si>
+  <si>
+    <t>stimulation</t>
+  </si>
+  <si>
+    <t>/ˌstɪmjuˈleɪʃ(ə)n/</t>
+  </si>
+  <si>
+    <t>simulation</t>
+  </si>
+  <si>
+    <t>/ˌsɪmjuˈleɪʃ(ə)n/</t>
+  </si>
+  <si>
+    <t>affair</t>
+  </si>
+  <si>
+    <t>/əˈfer/</t>
+  </si>
+  <si>
+    <t>expert</t>
+  </si>
+  <si>
+    <t>/ˈekspɜːrt/</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>/ˈwiːkdeɪ/</t>
+  </si>
+  <si>
+    <t>weekend</t>
+  </si>
+  <si>
+    <t>/ˈwiːkend/</t>
+  </si>
+  <si>
+    <t>overturn</t>
+  </si>
+  <si>
+    <t>/ˌoʊvərˈtɜːrn/</t>
+  </si>
+  <si>
+    <t>despite</t>
+  </si>
+  <si>
+    <t>/dɪˈspaɪt/</t>
+  </si>
+  <si>
     <t>Phrase</t>
   </si>
   <si>
@@ -748,6 +949,15 @@
   </si>
   <si>
     <t>Starship with humans for scale.</t>
+  </si>
+  <si>
+    <t>put on hold</t>
+  </si>
+  <si>
+    <t>搁置、延期、暂停</t>
+  </si>
+  <si>
+    <t>President Trump has said he doesn't want a "wasted meeting" after plans for a summit on Ukraine with Vladimir Putin in Bucharest were put on hold.</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1585,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1390,6 +1600,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1924,15 +2137,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2082,6 +2295,275 @@
       </c>
       <c r="B20" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:2">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>93</v>
+      </c>
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2093,12 +2575,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -2111,753 +2593,764 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" ht="14.25" spans="1:3">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>82</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>151</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" ht="14.25" spans="1:4">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>155</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>89</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>165</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>171</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>172</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>177</v>
       </c>
       <c r="D26" t="s">
-        <v>111</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>182</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>185</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>122</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>194</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>196</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>197</v>
       </c>
       <c r="C33" t="s">
-        <v>131</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>202</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>203</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" ht="40.5" spans="1:4">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>139</v>
+        <v>206</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>208</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>209</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="B39" t="s">
-        <v>147</v>
+        <v>214</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>216</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>217</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>152</v>
+        <v>219</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>220</v>
       </c>
       <c r="C41" t="s">
-        <v>154</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>155</v>
+        <v>222</v>
       </c>
       <c r="B42" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>157</v>
+        <v>224</v>
       </c>
       <c r="B43" t="s">
-        <v>158</v>
+        <v>225</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>226</v>
       </c>
       <c r="D43" t="s">
-        <v>160</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>229</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>230</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" ht="27" spans="1:4">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
       <c r="C45" t="s">
-        <v>167</v>
+        <v>234</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>168</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>238</v>
       </c>
       <c r="B47" t="s">
-        <v>172</v>
+        <v>239</v>
       </c>
       <c r="C47" t="s">
-        <v>173</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>241</v>
       </c>
       <c r="B48" t="s">
-        <v>175</v>
+        <v>242</v>
       </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>243</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>245</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>179</v>
+        <v>246</v>
       </c>
       <c r="B50" t="s">
-        <v>180</v>
+        <v>247</v>
       </c>
       <c r="C50" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
       <c r="B51" t="s">
-        <v>183</v>
+        <v>250</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>252</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>253</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>187</v>
+        <v>254</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>255</v>
       </c>
       <c r="B53" t="s">
-        <v>189</v>
+        <v>256</v>
       </c>
       <c r="D53" t="s">
-        <v>190</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>191</v>
+        <v>258</v>
       </c>
       <c r="B54" t="s">
-        <v>192</v>
+        <v>259</v>
       </c>
       <c r="C54" t="s">
-        <v>193</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>262</v>
       </c>
       <c r="D55" t="s">
-        <v>196</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>197</v>
+        <v>264</v>
       </c>
       <c r="B56" t="s">
-        <v>198</v>
+        <v>265</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>199</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>200</v>
+        <v>267</v>
       </c>
       <c r="B57" t="s">
-        <v>201</v>
+        <v>268</v>
       </c>
       <c r="C57" t="s">
-        <v>202</v>
+        <v>269</v>
       </c>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>204</v>
+        <v>271</v>
       </c>
       <c r="B58" t="s">
-        <v>205</v>
+        <v>272</v>
       </c>
       <c r="C58" t="s">
-        <v>206</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>207</v>
+        <v>274</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>275</v>
       </c>
       <c r="D59" t="s">
-        <v>209</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>210</v>
+        <v>277</v>
       </c>
       <c r="B60" t="s">
-        <v>211</v>
+        <v>278</v>
       </c>
       <c r="D60" t="s">
-        <v>212</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>213</v>
+        <v>280</v>
       </c>
       <c r="B61" t="s">
-        <v>214</v>
+        <v>281</v>
       </c>
       <c r="D61" t="s">
-        <v>215</v>
+        <v>282</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>216</v>
+        <v>283</v>
       </c>
       <c r="B62" t="s">
-        <v>217</v>
+        <v>284</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>218</v>
+        <v>285</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>286</v>
       </c>
       <c r="C63" t="s">
-        <v>220</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>221</v>
+        <v>288</v>
       </c>
       <c r="B64" t="s">
-        <v>222</v>
+        <v>289</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>223</v>
+        <v>290</v>
       </c>
       <c r="B65" t="s">
-        <v>224</v>
+        <v>291</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>225</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>226</v>
+        <v>293</v>
       </c>
       <c r="B66" t="s">
-        <v>227</v>
+        <v>294</v>
       </c>
       <c r="D66" t="s">
-        <v>228</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>229</v>
+        <v>296</v>
       </c>
       <c r="B67" t="s">
-        <v>230</v>
+        <v>297</v>
       </c>
       <c r="C67" t="s">
-        <v>231</v>
+        <v>298</v>
       </c>
       <c r="D67" t="s">
-        <v>232</v>
+        <v>299</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>233</v>
+        <v>300</v>
       </c>
       <c r="B68" t="s">
-        <v>234</v>
+        <v>301</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>235</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>236</v>
+        <v>303</v>
       </c>
       <c r="B69" t="s">
-        <v>237</v>
+        <v>304</v>
       </c>
       <c r="C69" t="s">
-        <v>238</v>
+        <v>305</v>
       </c>
       <c r="D69" t="s">
-        <v>239</v>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>307</v>
+      </c>
+      <c r="B70" t="s">
+        <v>308</v>
+      </c>
+      <c r="D70" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
css: add CSS values and units and sizing items
</commit_message>
<xml_diff>
--- a/english/phrases.xlsx
+++ b/english/phrases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255"/>
+    <workbookView windowWidth="27945" windowHeight="12255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="word" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="349">
   <si>
     <t>word</t>
   </si>
@@ -378,6 +378,48 @@
     <t>/ˈvɜːrsəs/</t>
   </si>
   <si>
+    <t>opaque</t>
+  </si>
+  <si>
+    <t>/oʊˈpeɪk/</t>
+  </si>
+  <si>
+    <t>opacity</t>
+  </si>
+  <si>
+    <t>/oʊˈpæsəti/</t>
+  </si>
+  <si>
+    <t>finite</t>
+  </si>
+  <si>
+    <t>/ˈfaɪnaɪt/</t>
+  </si>
+  <si>
+    <t>infinite</t>
+  </si>
+  <si>
+    <t>/ˈɪnfɪnət/</t>
+  </si>
+  <si>
+    <t>align</t>
+  </si>
+  <si>
+    <t>/əˈlaɪn/</t>
+  </si>
+  <si>
+    <t>intrinsic</t>
+  </si>
+  <si>
+    <t>/ɪnˈtrɪnzɪk/</t>
+  </si>
+  <si>
+    <t>extrinsic</t>
+  </si>
+  <si>
+    <t>/ɪksˈtrɪnzɪk/</t>
+  </si>
+  <si>
     <t>Phrase</t>
   </si>
   <si>
@@ -1015,6 +1057,24 @@
   </si>
   <si>
     <t>The following table shows a few isolated examples to get you in the mood.</t>
+  </si>
+  <si>
+    <t>over and over</t>
+  </si>
+  <si>
+    <t>反复、再三、一次又一次</t>
+  </si>
+  <si>
+    <t>In programming, a function is a piece of code that does a specific task. Functions are useful because you can write code once then reuse it many times instead of writing the same logic over and over.</t>
+  </si>
+  <si>
+    <t>scale down</t>
+  </si>
+  <si>
+    <t>按比例缩小</t>
+  </si>
+  <si>
+    <t>A common use of max-width is to cause images to scale down if there is not enough space to display them at their intrinsic width, while making sure they don't become larger than that width.</t>
   </si>
 </sst>
 </file>
@@ -2191,10 +2251,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -2665,6 +2725,62 @@
       </c>
       <c r="B58" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2679,12 +2795,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -2697,786 +2813,808 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" spans="1:3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:4">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="B18" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" ht="14.25" spans="1:4">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="B20" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="B22" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="B24" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="C24" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="D24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="B26" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="D26" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="B28" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="C28" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" ht="15" spans="1:3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:4">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>199</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="D30" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="B32" t="s">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="C32" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="D32" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="B33" t="s">
-        <v>210</v>
+        <v>224</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>212</v>
+        <v>226</v>
       </c>
       <c r="B34" t="s">
-        <v>213</v>
+        <v>227</v>
       </c>
       <c r="C34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" ht="40.5" spans="1:4">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="B36" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="B37" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="B38" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="B39" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="C39" t="s">
-        <v>228</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="D40" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B41" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="C41" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>249</v>
       </c>
       <c r="B42" t="s">
-        <v>236</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>237</v>
+        <v>251</v>
       </c>
       <c r="B43" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="C43" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="D43" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="B44" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="C44" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="D44" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" ht="27" spans="1:4">
       <c r="A45" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="B45" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="C45" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="B46" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B47" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="C47" t="s">
-        <v>253</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="B48" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="D48" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="B49" t="s">
-        <v>258</v>
+        <v>272</v>
       </c>
       <c r="D49" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="B50" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B51" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="C51" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="B52" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="C52" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="53" ht="15" spans="1:3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="53" ht="15" spans="1:4">
       <c r="A53" t="s">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="B53" t="s">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>270</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="B54" t="s">
-        <v>272</v>
+        <v>286</v>
       </c>
       <c r="D54" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="B55" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="C55" t="s">
-        <v>276</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="B56" t="s">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="D56" t="s">
-        <v>279</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B57" t="s">
-        <v>281</v>
+        <v>295</v>
       </c>
       <c r="D57" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="B58" t="s">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B59" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="C59" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="D59" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="B60" t="s">
-        <v>291</v>
+        <v>305</v>
       </c>
       <c r="C60" t="s">
-        <v>292</v>
+        <v>306</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="B61" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="D61" t="s">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="B62" t="s">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="D62" t="s">
-        <v>298</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="B63" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
       <c r="D63" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>302</v>
+        <v>316</v>
       </c>
       <c r="B64" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>304</v>
+        <v>318</v>
       </c>
       <c r="B65" t="s">
-        <v>305</v>
+        <v>319</v>
       </c>
       <c r="C65" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="B66" t="s">
-        <v>308</v>
+        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>309</v>
+        <v>323</v>
       </c>
       <c r="B67" t="s">
-        <v>310</v>
+        <v>324</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="B68" t="s">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="D68" t="s">
-        <v>314</v>
+        <v>328</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="B69" t="s">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="C69" t="s">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="D69" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>319</v>
+        <v>333</v>
       </c>
       <c r="B70" t="s">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>321</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="B71" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="C71" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="D71" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>326</v>
+        <v>340</v>
       </c>
       <c r="B72" t="s">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="D72" t="s">
-        <v>328</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>343</v>
+      </c>
+      <c r="B73" t="s">
+        <v>344</v>
+      </c>
+      <c r="D73" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>346</v>
+      </c>
+      <c r="B74" t="s">
+        <v>347</v>
+      </c>
+      <c r="D74" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
frontend/css: add overflow and refine
</commit_message>
<xml_diff>
--- a/english/phrases.xlsx
+++ b/english/phrases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12255" activeTab="1"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="word" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="381">
   <si>
     <t>word</t>
   </si>
@@ -72,6 +72,18 @@
     <t>/əˈses/</t>
   </si>
   <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>/əˈsaɪn/</t>
+  </si>
+  <si>
+    <t>axis</t>
+  </si>
+  <si>
+    <t>/ˈæksɪs/</t>
+  </si>
+  <si>
     <t>bind</t>
   </si>
   <si>
@@ -120,6 +132,12 @@
     <t>/kənˈsɜːrv/</t>
   </si>
   <si>
+    <t>convict</t>
+  </si>
+  <si>
+    <t>/kənˈvɪkt/</t>
+  </si>
+  <si>
     <t>create</t>
   </si>
   <si>
@@ -144,6 +162,12 @@
     <t>/det/</t>
   </si>
   <si>
+    <t>democratic</t>
+  </si>
+  <si>
+    <t>/ˌdeməˈkrætɪk/</t>
+  </si>
+  <si>
     <t>descendant</t>
   </si>
   <si>
@@ -516,7 +540,7 @@
     <t>正如、与…一样、就…来说</t>
   </si>
   <si>
-    <t>As with any shorthand property, any individual value that is not specified is set to its corresponding initial value</t>
+    <t>As with any shorthand property, any individual value that is not specified is set to its corresponding initial value.</t>
   </si>
   <si>
     <t>at the speed of</t>
@@ -2323,10 +2347,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -2395,15 +2419,15 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="14.25" spans="1:2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2411,15 +2435,15 @@
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" ht="14.25" spans="1:2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2463,19 +2487,19 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" ht="15" spans="1:2">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="15" spans="1:2">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2487,19 +2511,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" ht="15" spans="1:2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" ht="15" spans="1:2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2583,11 +2607,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" ht="15" spans="1:2">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2647,11 +2671,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" ht="15" spans="1:2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2675,7 +2699,7 @@
       <c r="A43" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2687,11 +2711,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="45" ht="15" spans="1:2">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2707,7 +2731,7 @@
       <c r="A47" t="s">
         <v>92</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2719,19 +2743,19 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" ht="15" spans="1:2">
       <c r="A49" t="s">
         <v>96</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="50" ht="15" spans="1:2">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2759,11 +2783,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" ht="15" spans="1:2">
       <c r="A54" t="s">
         <v>106</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2815,11 +2839,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="61" ht="15" spans="1:2">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2831,11 +2855,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" ht="14.25" spans="1:2">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2847,11 +2871,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" ht="15" spans="1:2">
       <c r="A65" t="s">
         <v>128</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2863,11 +2887,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" ht="14.25" spans="1:2">
       <c r="A67" t="s">
         <v>132</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2876,28 +2900,60 @@
         <v>134</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>143</v>
+      </c>
+      <c r="B73" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>145</v>
+      </c>
+      <c r="B74" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B70">
-    <sortCondition ref="A2:A70"/>
+  <sortState ref="A2:B74">
+    <sortCondition ref="A2:A74"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2909,10 +2965,10 @@
   <sheetPr/>
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D78"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -2925,861 +2981,861 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B14" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B17" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D17" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B18" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" ht="14.25" spans="1:4">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B20" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B21" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" ht="14.25" spans="1:4">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="C23" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B24" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="C24" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B25" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="D25" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B26" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C27" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="D27" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D29" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B30" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C31" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:4">
       <c r="A32" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B32" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="B33" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="D33" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B34" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B35" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D35" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B36" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="D36" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B37" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C37" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B38" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C38" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B39" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C39" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="40" ht="40.5" spans="1:4">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B40" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C41" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B42" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="B43" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C43" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D43" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B44" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="D44" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="B45" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="C45" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="B46" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="B47" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C47" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="D47" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="C48" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="D48" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" ht="27" spans="1:4">
       <c r="A49" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="B49" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C49" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B50" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="D50" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="B51" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="B52" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="C52" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="B53" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="D53" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="B54" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="D54" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C56" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="B57" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="C57" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:4">
       <c r="A58" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="B59" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="D59" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="B60" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C60" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="B61" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="D61" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="B62" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="D62" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="B63" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="D63" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="B64" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="B65" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="C65" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="D65" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="B66" t="s">
-        <v>334</v>
+        <v>342</v>
       </c>
       <c r="C66" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B67" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="D67" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>339</v>
+        <v>347</v>
       </c>
       <c r="B68" t="s">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="C68" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="D68" t="s">
-        <v>342</v>
+        <v>350</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="B69" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
       <c r="D69" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>346</v>
+        <v>354</v>
       </c>
       <c r="B70" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="D70" t="s">
-        <v>348</v>
+        <v>356</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>349</v>
+        <v>357</v>
       </c>
       <c r="B71" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>351</v>
+        <v>359</v>
       </c>
       <c r="B72" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C72" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="B73" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>356</v>
+        <v>364</v>
       </c>
       <c r="B74" t="s">
-        <v>357</v>
+        <v>365</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="B75" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="D75" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="B76" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="C76" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="D76" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="B77" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="B78" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="C78" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
       <c r="D78" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
frontend/css: add images、media and form elements
</commit_message>
<xml_diff>
--- a/english/phrases.xlsx
+++ b/english/phrases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="393">
   <si>
     <t>word</t>
   </si>
@@ -471,6 +471,18 @@
     <t>/ˈwiːkend/</t>
   </si>
   <si>
+    <t>bounty</t>
+  </si>
+  <si>
+    <t>/ˈbaʊnti/</t>
+  </si>
+  <si>
+    <t>distort</t>
+  </si>
+  <si>
+    <t>/dɪˈstɔːrt/</t>
+  </si>
+  <si>
     <t>Phrase</t>
   </si>
   <si>
@@ -1171,6 +1183,30 @@
   </si>
   <si>
     <t>Starship with humans for scale.</t>
+  </si>
+  <si>
+    <t>be intended for</t>
+  </si>
+  <si>
+    <t>被设计给/被用来给/是为了…而准备的</t>
+  </si>
+  <si>
+    <t>表示某物的预期用途、目标用户或目的。</t>
+  </si>
+  <si>
+    <t>MySQL Server is intended for mission-critical, heavy-load production systems as well as for embedding into mass-deployed software.</t>
+  </si>
+  <si>
+    <t>work toward</t>
+  </si>
+  <si>
+    <t>朝着某个方向努力、逐步实现</t>
+  </si>
+  <si>
+    <t>强调这是一个进行中的、有意识的目标，而不是已经完成的状态。</t>
+  </si>
+  <si>
+    <t>One of our main goals with the product is to continue to work toward compliance with the SQL standard, but without sacrificing speed or reliability.</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1214,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1653,19 +1689,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2347,10 +2383,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -2949,6 +2985,22 @@
       </c>
       <c r="B74" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B75" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B76" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2963,12 +3015,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -2981,861 +3033,889 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C13" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" ht="14.25" spans="1:4">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C19" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" ht="14.25" spans="1:4">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C22" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B23" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C23" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B24" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C24" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="B25" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D25" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="B26" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B27" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="C27" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D27" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="B28" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B29" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D29" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="B30" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B31" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:4">
       <c r="A32" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="B32" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="B33" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D33" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B34" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C35" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D35" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B36" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="D36" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B37" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C37" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="B38" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C38" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B39" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="C39" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" ht="40.5" spans="1:4">
       <c r="A40" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B40" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B41" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B42" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B43" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C43" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D43" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B44" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D44" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B45" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C45" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B46" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B47" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C47" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D47" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B48" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C48" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="D48" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" ht="27" spans="1:4">
       <c r="A49" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B49" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C49" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D50" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B51" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B52" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="C52" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="D53" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B54" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D54" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B55" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B56" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C56" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="B57" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="C57" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:4">
       <c r="A58" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B58" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="B59" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="D59" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C60" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B61" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="D61" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="B62" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D62" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B63" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="D63" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="B64" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B65" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C65" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D65" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="B66" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C66" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B67" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="D67" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B68" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C68" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="D68" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B69" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="D69" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="B70" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="D70" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="B71" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="B72" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C72" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B73" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B74" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B75" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="D75" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="B76" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="C76" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="D76" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B77" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B78" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C78" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="D78" t="s">
-        <v>380</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>385</v>
+      </c>
+      <c r="B79" t="s">
+        <v>386</v>
+      </c>
+      <c r="C79" t="s">
+        <v>387</v>
+      </c>
+      <c r="D79" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>389</v>
+      </c>
+      <c r="B80" t="s">
+        <v>390</v>
+      </c>
+      <c r="C80" t="s">
+        <v>391</v>
+      </c>
+      <c r="D80" t="s">
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>